<commit_message>
not set style for normal data
</commit_message>
<xml_diff>
--- a/test.data.xlsx
+++ b/test.data.xlsx
@@ -31,7 +31,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -47,10 +47,7 @@
     <font>
       <name val="Arial"/>
       <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="4">
@@ -83,11 +80,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -104,15 +100,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
     </row>

</xml_diff>